<commit_message>
Biplots highlighting P2O5 zero_values data
</commit_message>
<xml_diff>
--- a/_BIPLOTS/area4.xlsx
+++ b/_BIPLOTS/area4.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG3" t="n">
@@ -868,7 +868,7 @@
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG4" t="n">
@@ -985,7 +985,7 @@
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG5" t="n">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG6" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG7" t="n">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG8" t="n">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG10" t="n">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG12" t="n">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG13" t="n">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG14" t="n">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG16" t="n">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG17" t="n">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG18" t="n">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG20" t="n">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG21" t="n">
@@ -2958,7 +2958,7 @@
       </c>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG22" t="n">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="AF24" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG24" t="n">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG25" t="n">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG28" t="n">
@@ -3761,7 +3761,7 @@
       </c>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG29" t="n">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG30" t="n">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG31" t="n">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG33" t="n">
@@ -4346,7 +4346,7 @@
       </c>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG34" t="n">
@@ -4580,7 +4580,7 @@
       </c>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG36" t="n">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG37" t="n">
@@ -4814,7 +4814,7 @@
       </c>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG38" t="n">
@@ -4931,7 +4931,7 @@
       </c>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG39" t="n">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="AF41" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG41" t="n">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="AF42" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG42" t="n">
@@ -5395,7 +5395,7 @@
       </c>
       <c r="AF43" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG43" t="n">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="AF45" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG45" t="n">
@@ -5867,7 +5867,7 @@
       </c>
       <c r="AF47" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG47" t="n">
@@ -6093,7 +6093,7 @@
       </c>
       <c r="AF49" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG49" t="n">
@@ -6210,7 +6210,7 @@
       </c>
       <c r="AF50" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG50" t="n">
@@ -6331,7 +6331,7 @@
       </c>
       <c r="AF51" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>mineralP2O5</t>
         </is>
       </c>
       <c r="AG51" t="n">
@@ -6444,7 +6444,7 @@
       </c>
       <c r="AF52" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG52" t="n">
@@ -6912,7 +6912,7 @@
       </c>
       <c r="AF56" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG56" t="n">
@@ -7150,7 +7150,7 @@
       </c>
       <c r="AF58" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG58" t="n">
@@ -7271,7 +7271,7 @@
       </c>
       <c r="AF59" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG59" t="n">
@@ -7388,7 +7388,7 @@
       </c>
       <c r="AF60" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG60" t="n">
@@ -7622,7 +7622,7 @@
       </c>
       <c r="AF62" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG62" t="n">
@@ -7735,7 +7735,7 @@
       </c>
       <c r="AF63" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG63" t="n">
@@ -7856,7 +7856,7 @@
       </c>
       <c r="AF64" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG64" t="n">
@@ -7969,7 +7969,7 @@
       </c>
       <c r="AF65" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG65" t="n">
@@ -8086,7 +8086,7 @@
       </c>
       <c r="AF66" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG66" t="n">
@@ -8195,7 +8195,7 @@
       </c>
       <c r="AF67" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG67" t="n">
@@ -8308,7 +8308,7 @@
       </c>
       <c r="AF68" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG68" t="n">
@@ -8429,7 +8429,7 @@
       </c>
       <c r="AF69" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG69" t="n">
@@ -8546,7 +8546,7 @@
       </c>
       <c r="AF70" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG70" t="n">
@@ -8667,7 +8667,7 @@
       </c>
       <c r="AF71" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG71" t="n">
@@ -8784,7 +8784,7 @@
       </c>
       <c r="AF72" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG72" t="n">
@@ -8905,7 +8905,7 @@
       </c>
       <c r="AF73" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG73" t="n">
@@ -9018,7 +9018,7 @@
       </c>
       <c r="AF74" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG74" t="n">
@@ -9127,7 +9127,7 @@
       </c>
       <c r="AF75" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG75" t="n">
@@ -9240,7 +9240,7 @@
       </c>
       <c r="AF76" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG76" t="n">
@@ -9353,7 +9353,7 @@
       </c>
       <c r="AF77" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG77" t="n">
@@ -9821,7 +9821,7 @@
       </c>
       <c r="AF81" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG81" t="n">
@@ -10055,7 +10055,7 @@
       </c>
       <c r="AF83" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG83" t="n">
@@ -10293,7 +10293,7 @@
       </c>
       <c r="AF85" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG85" t="n">
@@ -10414,7 +10414,7 @@
       </c>
       <c r="AF86" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG86" t="n">
@@ -10527,7 +10527,7 @@
       </c>
       <c r="AF87" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG87" t="n">
@@ -10640,7 +10640,7 @@
       </c>
       <c r="AF88" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG88" t="n">
@@ -10749,7 +10749,7 @@
       </c>
       <c r="AF89" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG89" t="n">
@@ -10858,7 +10858,7 @@
       </c>
       <c r="AF90" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG90" t="n">
@@ -10975,7 +10975,7 @@
       </c>
       <c r="AF91" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG91" t="n">
@@ -11201,7 +11201,7 @@
       </c>
       <c r="AF93" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG93" t="n">
@@ -11314,7 +11314,7 @@
       </c>
       <c r="AF94" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG94" t="n">
@@ -11431,7 +11431,7 @@
       </c>
       <c r="AF95" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>mineralP2O5</t>
         </is>
       </c>
       <c r="AG95" t="n">
@@ -11544,7 +11544,7 @@
       </c>
       <c r="AF96" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG96" t="n">
@@ -11665,7 +11665,7 @@
       </c>
       <c r="AF97" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG97" t="n">
@@ -11899,7 +11899,7 @@
       </c>
       <c r="AF99" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG99" t="n">
@@ -12020,7 +12020,7 @@
       </c>
       <c r="AF100" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG100" t="n">
@@ -12141,7 +12141,7 @@
       </c>
       <c r="AF101" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG101" t="n">
@@ -12262,7 +12262,7 @@
       </c>
       <c r="AF102" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG102" t="n">
@@ -12375,7 +12375,7 @@
       </c>
       <c r="AF103" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG103" t="n">
@@ -12492,7 +12492,7 @@
       </c>
       <c r="AF104" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG104" t="n">
@@ -12605,7 +12605,7 @@
       </c>
       <c r="AF105" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG105" t="n">
@@ -12722,7 +12722,7 @@
       </c>
       <c r="AF106" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG106" t="n">
@@ -12839,7 +12839,7 @@
       </c>
       <c r="AF107" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG107" t="n">
@@ -12960,7 +12960,7 @@
       </c>
       <c r="AF108" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG108" t="n">
@@ -13077,7 +13077,7 @@
       </c>
       <c r="AF109" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG109" t="n">
@@ -13190,7 +13190,7 @@
       </c>
       <c r="AF110" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG110" t="n">
@@ -13299,7 +13299,7 @@
       </c>
       <c r="AF111" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG111" t="n">
@@ -13416,7 +13416,7 @@
       </c>
       <c r="AF112" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG112" t="n">
@@ -13529,7 +13529,7 @@
       </c>
       <c r="AF113" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG113" t="n">
@@ -13646,7 +13646,7 @@
       </c>
       <c r="AF114" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG114" t="n">
@@ -13767,7 +13767,7 @@
       </c>
       <c r="AF115" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG115" t="n">
@@ -13888,7 +13888,7 @@
       </c>
       <c r="AF116" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG116" t="n">
@@ -14005,7 +14005,7 @@
       </c>
       <c r="AF117" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG117" t="n">
@@ -14122,7 +14122,7 @@
       </c>
       <c r="AF118" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG118" t="n">
@@ -14239,7 +14239,7 @@
       </c>
       <c r="AF119" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG119" t="n">
@@ -14352,7 +14352,7 @@
       </c>
       <c r="AF120" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG120" t="n">
@@ -14473,7 +14473,7 @@
       </c>
       <c r="AF121" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG121" t="n">
@@ -14828,7 +14828,7 @@
       </c>
       <c r="AF124" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG124" t="n">
@@ -14941,7 +14941,7 @@
       </c>
       <c r="AF125" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG125" t="n">
@@ -15050,7 +15050,7 @@
       </c>
       <c r="AF126" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG126" t="n">
@@ -15167,7 +15167,7 @@
       </c>
       <c r="AF127" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG127" t="n">
@@ -15276,7 +15276,7 @@
       </c>
       <c r="AF128" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG128" t="n">
@@ -15518,7 +15518,7 @@
       </c>
       <c r="AF130" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG130" t="n">
@@ -15631,7 +15631,7 @@
       </c>
       <c r="AF131" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG131" t="n">
@@ -15748,7 +15748,7 @@
       </c>
       <c r="AF132" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG132" t="n">
@@ -15861,7 +15861,7 @@
       </c>
       <c r="AF133" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG133" t="n">
@@ -15970,7 +15970,7 @@
       </c>
       <c r="AF134" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG134" t="n">
@@ -16091,7 +16091,7 @@
       </c>
       <c r="AF135" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG135" t="n">
@@ -16204,7 +16204,7 @@
       </c>
       <c r="AF136" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG136" t="n">
@@ -16321,7 +16321,7 @@
       </c>
       <c r="AF137" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG137" t="n">
@@ -16547,7 +16547,7 @@
       </c>
       <c r="AF139" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG139" t="n">
@@ -16785,7 +16785,7 @@
       </c>
       <c r="AF141" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG141" t="n">
@@ -16898,7 +16898,7 @@
       </c>
       <c r="AF142" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG142" t="n">
@@ -17019,7 +17019,7 @@
       </c>
       <c r="AF143" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG143" t="n">
@@ -17249,7 +17249,7 @@
       </c>
       <c r="AF145" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG145" t="n">
@@ -17362,7 +17362,7 @@
       </c>
       <c r="AF146" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG146" t="n">
@@ -17475,7 +17475,7 @@
       </c>
       <c r="AF147" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG147" t="n">
@@ -17588,7 +17588,7 @@
       </c>
       <c r="AF148" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG148" t="n">
@@ -17701,7 +17701,7 @@
       </c>
       <c r="AF149" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG149" t="n">
@@ -18181,7 +18181,7 @@
       </c>
       <c r="AF153" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG153" t="n">
@@ -18294,7 +18294,7 @@
       </c>
       <c r="AF154" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG154" t="n">
@@ -18649,7 +18649,7 @@
       </c>
       <c r="AF157" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG157" t="n">
@@ -18762,7 +18762,7 @@
       </c>
       <c r="AF158" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG158" t="n">
@@ -18871,7 +18871,7 @@
       </c>
       <c r="AF159" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG159" t="n">
@@ -19230,7 +19230,7 @@
       </c>
       <c r="AF162" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG162" t="n">
@@ -19468,7 +19468,7 @@
       </c>
       <c r="AF164" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG164" t="n">
@@ -19581,7 +19581,7 @@
       </c>
       <c r="AF165" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG165" t="n">
@@ -19698,7 +19698,7 @@
       </c>
       <c r="AF166" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG166" t="n">
@@ -19924,7 +19924,7 @@
       </c>
       <c r="AF168" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG168" t="n">
@@ -20037,7 +20037,7 @@
       </c>
       <c r="AF169" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG169" t="n">
@@ -20154,7 +20154,7 @@
       </c>
       <c r="AF170" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG170" t="n">
@@ -20388,7 +20388,7 @@
       </c>
       <c r="AF172" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG172" t="n">
@@ -20505,7 +20505,7 @@
       </c>
       <c r="AF173" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG173" t="n">
@@ -20626,7 +20626,7 @@
       </c>
       <c r="AF174" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG174" t="n">
@@ -21090,7 +21090,7 @@
       </c>
       <c r="AF178" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG178" t="n">
@@ -21207,7 +21207,7 @@
       </c>
       <c r="AF179" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG179" t="n">
@@ -21437,7 +21437,7 @@
       </c>
       <c r="AF181" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG181" t="n">
@@ -21667,7 +21667,7 @@
       </c>
       <c r="AF183" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG183" t="n">
@@ -21780,7 +21780,7 @@
       </c>
       <c r="AF184" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG184" t="n">
@@ -22018,7 +22018,7 @@
       </c>
       <c r="AF186" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG186" t="n">
@@ -22486,7 +22486,7 @@
       </c>
       <c r="AF190" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG190" t="n">
@@ -22603,7 +22603,7 @@
       </c>
       <c r="AF191" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG191" t="n">
@@ -23192,7 +23192,7 @@
       </c>
       <c r="AF196" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG196" t="n">
@@ -23301,7 +23301,7 @@
       </c>
       <c r="AF197" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG197" t="n">
@@ -23414,7 +23414,7 @@
       </c>
       <c r="AF198" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG198" t="n">
@@ -23535,7 +23535,7 @@
       </c>
       <c r="AF199" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG199" t="n">
@@ -23882,7 +23882,7 @@
       </c>
       <c r="AF202" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG202" t="n">
@@ -24221,7 +24221,7 @@
       </c>
       <c r="AF205" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG205" t="n">
@@ -24334,7 +24334,7 @@
       </c>
       <c r="AF206" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG206" t="n">
@@ -24447,7 +24447,7 @@
       </c>
       <c r="AF207" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG207" t="n">
@@ -24564,7 +24564,7 @@
       </c>
       <c r="AF208" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG208" t="n">
@@ -24677,7 +24677,7 @@
       </c>
       <c r="AF209" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG209" t="n">
@@ -24794,7 +24794,7 @@
       </c>
       <c r="AF210" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG210" t="n">
@@ -24907,7 +24907,7 @@
       </c>
       <c r="AF211" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG211" t="n">
@@ -25024,7 +25024,7 @@
       </c>
       <c r="AF212" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG212" t="n">
@@ -25141,7 +25141,7 @@
       </c>
       <c r="AF213" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG213" t="n">
@@ -25254,7 +25254,7 @@
       </c>
       <c r="AF214" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG214" t="n">
@@ -25371,7 +25371,7 @@
       </c>
       <c r="AF215" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG215" t="n">
@@ -25605,7 +25605,7 @@
       </c>
       <c r="AF217" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG217" t="n">
@@ -25847,7 +25847,7 @@
       </c>
       <c r="AF219" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG219" t="n">
@@ -26085,7 +26085,7 @@
       </c>
       <c r="AF221" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG221" t="n">
@@ -26198,7 +26198,7 @@
       </c>
       <c r="AF222" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG222" t="n">
@@ -26424,7 +26424,7 @@
       </c>
       <c r="AF224" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG224" t="n">
@@ -26654,7 +26654,7 @@
       </c>
       <c r="AF226" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG226" t="n">
@@ -26767,7 +26767,7 @@
       </c>
       <c r="AF227" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG227" t="n">
@@ -26880,7 +26880,7 @@
       </c>
       <c r="AF228" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG228" t="n">
@@ -27110,7 +27110,7 @@
       </c>
       <c r="AF230" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG230" t="n">
@@ -27219,7 +27219,7 @@
       </c>
       <c r="AF231" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG231" t="n">
@@ -27675,7 +27675,7 @@
       </c>
       <c r="AF235" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG235" t="n">
@@ -27905,7 +27905,7 @@
       </c>
       <c r="AF237" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG237" t="n">
@@ -28022,7 +28022,7 @@
       </c>
       <c r="AF238" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG238" t="n">
@@ -28135,7 +28135,7 @@
       </c>
       <c r="AF239" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG239" t="n">
@@ -28248,7 +28248,7 @@
       </c>
       <c r="AF240" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG240" t="n">
@@ -28361,7 +28361,7 @@
       </c>
       <c r="AF241" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG241" t="n">
@@ -28474,7 +28474,7 @@
       </c>
       <c r="AF242" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG242" t="n">
@@ -28708,7 +28708,7 @@
       </c>
       <c r="AF244" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG244" t="n">
@@ -28946,7 +28946,7 @@
       </c>
       <c r="AF246" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG246" t="n">
@@ -29527,7 +29527,7 @@
       </c>
       <c r="AF251" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG251" t="n">
@@ -29640,7 +29640,7 @@
       </c>
       <c r="AF252" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG252" t="n">
@@ -29753,7 +29753,7 @@
       </c>
       <c r="AF253" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG253" t="n">
@@ -29866,7 +29866,7 @@
       </c>
       <c r="AF254" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG254" t="n">
@@ -29979,7 +29979,7 @@
       </c>
       <c r="AF255" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG255" t="n">
@@ -30096,7 +30096,7 @@
       </c>
       <c r="AF256" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG256" t="n">
@@ -30334,7 +30334,7 @@
       </c>
       <c r="AF258" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG258" t="n">
@@ -30447,7 +30447,7 @@
       </c>
       <c r="AF259" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG259" t="n">
@@ -30681,7 +30681,7 @@
       </c>
       <c r="AF261" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG261" t="n">
@@ -30794,7 +30794,7 @@
       </c>
       <c r="AF262" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG262" t="n">
@@ -30915,7 +30915,7 @@
       </c>
       <c r="AF263" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG263" t="n">
@@ -31032,7 +31032,7 @@
       </c>
       <c r="AF264" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG264" t="n">
@@ -31141,7 +31141,7 @@
       </c>
       <c r="AF265" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG265" t="n">
@@ -31254,7 +31254,7 @@
       </c>
       <c r="AF266" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG266" t="n">
@@ -31367,7 +31367,7 @@
       </c>
       <c r="AF267" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG267" t="n">
@@ -31484,7 +31484,7 @@
       </c>
       <c r="AF268" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG268" t="n">
@@ -31597,7 +31597,7 @@
       </c>
       <c r="AF269" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG269" t="n">
@@ -31944,7 +31944,7 @@
       </c>
       <c r="AF272" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG272" t="n">
@@ -32061,7 +32061,7 @@
       </c>
       <c r="AF273" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG273" t="n">
@@ -32174,7 +32174,7 @@
       </c>
       <c r="AF274" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG274" t="n">
@@ -32291,7 +32291,7 @@
       </c>
       <c r="AF275" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG275" t="n">
@@ -32408,7 +32408,7 @@
       </c>
       <c r="AF276" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG276" t="n">
@@ -32525,7 +32525,7 @@
       </c>
       <c r="AF277" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG277" t="n">
@@ -32638,7 +32638,7 @@
       </c>
       <c r="AF278" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG278" t="n">
@@ -32872,7 +32872,7 @@
       </c>
       <c r="AF280" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG280" t="n">
@@ -32989,7 +32989,7 @@
       </c>
       <c r="AF281" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG281" t="n">
@@ -33215,7 +33215,7 @@
       </c>
       <c r="AF283" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG283" t="n">
@@ -33328,7 +33328,7 @@
       </c>
       <c r="AF284" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG284" t="n">
@@ -33445,7 +33445,7 @@
       </c>
       <c r="AF285" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG285" t="n">
@@ -33679,7 +33679,7 @@
       </c>
       <c r="AF287" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG287" t="n">
@@ -33796,7 +33796,7 @@
       </c>
       <c r="AF288" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG288" t="n">
@@ -34034,7 +34034,7 @@
       </c>
       <c r="AF290" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG290" t="n">
@@ -34151,7 +34151,7 @@
       </c>
       <c r="AF291" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG291" t="n">
@@ -34268,7 +34268,7 @@
       </c>
       <c r="AF292" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG292" t="n">
@@ -34381,7 +34381,7 @@
       </c>
       <c r="AF293" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG293" t="n">
@@ -34974,7 +34974,7 @@
       </c>
       <c r="AF298" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG298" t="n">
@@ -35208,7 +35208,7 @@
       </c>
       <c r="AF300" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG300" t="n">
@@ -35442,7 +35442,7 @@
       </c>
       <c r="AF302" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG302" t="n">
@@ -35551,7 +35551,7 @@
       </c>
       <c r="AF303" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG303" t="n">
@@ -35664,7 +35664,7 @@
       </c>
       <c r="AF304" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG304" t="n">
@@ -35781,7 +35781,7 @@
       </c>
       <c r="AF305" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG305" t="n">
@@ -36128,7 +36128,7 @@
       </c>
       <c r="AF308" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG308" t="n">
@@ -36475,7 +36475,7 @@
       </c>
       <c r="AF311" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG311" t="n">
@@ -36588,7 +36588,7 @@
       </c>
       <c r="AF312" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG312" t="n">
@@ -36830,7 +36830,7 @@
       </c>
       <c r="AF314" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG314" t="n">
@@ -37060,7 +37060,7 @@
       </c>
       <c r="AF316" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG316" t="n">
@@ -37294,7 +37294,7 @@
       </c>
       <c r="AF318" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG318" t="n">
@@ -37407,7 +37407,7 @@
       </c>
       <c r="AF319" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG319" t="n">
@@ -37637,7 +37637,7 @@
       </c>
       <c r="AF321" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG321" t="n">
@@ -37750,7 +37750,7 @@
       </c>
       <c r="AF322" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG322" t="n">
@@ -37863,7 +37863,7 @@
       </c>
       <c r="AF323" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG323" t="n">
@@ -37972,7 +37972,7 @@
       </c>
       <c r="AF324" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG324" t="n">
@@ -38198,7 +38198,7 @@
       </c>
       <c r="AF326" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG326" t="n">
@@ -38432,7 +38432,7 @@
       </c>
       <c r="AF328" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG328" t="n">
@@ -38545,7 +38545,7 @@
       </c>
       <c r="AF329" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG329" t="n">
@@ -38654,7 +38654,7 @@
       </c>
       <c r="AF330" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG330" t="n">
@@ -39009,7 +39009,7 @@
       </c>
       <c r="AF333" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG333" t="n">
@@ -39126,7 +39126,7 @@
       </c>
       <c r="AF334" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG334" t="n">
@@ -39235,7 +39235,7 @@
       </c>
       <c r="AF335" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG335" t="n">
@@ -39465,7 +39465,7 @@
       </c>
       <c r="AF337" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG337" t="n">
@@ -39574,7 +39574,7 @@
       </c>
       <c r="AF338" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG338" t="n">
@@ -39691,7 +39691,7 @@
       </c>
       <c r="AF339" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG339" t="n">
@@ -39808,7 +39808,7 @@
       </c>
       <c r="AF340" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG340" t="n">
@@ -40389,7 +40389,7 @@
       </c>
       <c r="AF345" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>mineralP2O5</t>
         </is>
       </c>
       <c r="AG345" t="n">
@@ -40736,7 +40736,7 @@
       </c>
       <c r="AF348" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG348" t="n">
@@ -40845,7 +40845,7 @@
       </c>
       <c r="AF349" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG349" t="n">
@@ -41196,7 +41196,7 @@
       </c>
       <c r="AF352" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG352" t="n">
@@ -41317,7 +41317,7 @@
       </c>
       <c r="AF353" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG353" t="n">
@@ -41430,7 +41430,7 @@
       </c>
       <c r="AF354" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG354" t="n">
@@ -41547,7 +41547,7 @@
       </c>
       <c r="AF355" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG355" t="n">
@@ -41773,7 +41773,7 @@
       </c>
       <c r="AF357" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG357" t="n">
@@ -41886,7 +41886,7 @@
       </c>
       <c r="AF358" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG358" t="n">
@@ -42120,7 +42120,7 @@
       </c>
       <c r="AF360" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG360" t="n">
@@ -42237,7 +42237,7 @@
       </c>
       <c r="AF361" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG361" t="n">
@@ -42463,7 +42463,7 @@
       </c>
       <c r="AF363" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG363" t="n">
@@ -42572,7 +42572,7 @@
       </c>
       <c r="AF364" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG364" t="n">
@@ -42681,7 +42681,7 @@
       </c>
       <c r="AF365" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG365" t="n">
@@ -42798,7 +42798,7 @@
       </c>
       <c r="AF366" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG366" t="n">
@@ -42911,7 +42911,7 @@
       </c>
       <c r="AF367" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG367" t="n">
@@ -43028,7 +43028,7 @@
       </c>
       <c r="AF368" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG368" t="n">
@@ -43137,7 +43137,7 @@
       </c>
       <c r="AF369" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG369" t="n">
@@ -43250,7 +43250,7 @@
       </c>
       <c r="AF370" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG370" t="n">
@@ -43363,7 +43363,7 @@
       </c>
       <c r="AF371" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG371" t="n">
@@ -43476,7 +43476,7 @@
       </c>
       <c r="AF372" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG372" t="n">
@@ -43585,7 +43585,7 @@
       </c>
       <c r="AF373" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG373" t="n">
@@ -43694,7 +43694,7 @@
       </c>
       <c r="AF374" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG374" t="n">
@@ -43807,7 +43807,7 @@
       </c>
       <c r="AF375" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG375" t="n">
@@ -44037,7 +44037,7 @@
       </c>
       <c r="AF377" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG377" t="n">
@@ -44150,7 +44150,7 @@
       </c>
       <c r="AF378" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG378" t="n">
@@ -44267,7 +44267,7 @@
       </c>
       <c r="AF379" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG379" t="n">
@@ -44493,7 +44493,7 @@
       </c>
       <c r="AF381" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG381" t="n">
@@ -44719,7 +44719,7 @@
       </c>
       <c r="AF383" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG383" t="n">
@@ -44949,7 +44949,7 @@
       </c>
       <c r="AF385" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG385" t="n">
@@ -45183,7 +45183,7 @@
       </c>
       <c r="AF387" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG387" t="n">
@@ -45417,7 +45417,7 @@
       </c>
       <c r="AF389" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG389" t="n">
@@ -45655,7 +45655,7 @@
       </c>
       <c r="AF391" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG391" t="n">
@@ -45764,7 +45764,7 @@
       </c>
       <c r="AF392" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG392" t="n">
@@ -46111,7 +46111,7 @@
       </c>
       <c r="AF395" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG395" t="n">
@@ -46228,7 +46228,7 @@
       </c>
       <c r="AF396" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG396" t="n">
@@ -46337,7 +46337,7 @@
       </c>
       <c r="AF397" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG397" t="n">
@@ -46446,7 +46446,7 @@
       </c>
       <c r="AF398" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG398" t="n">
@@ -46559,7 +46559,7 @@
       </c>
       <c r="AF399" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG399" t="n">
@@ -46676,7 +46676,7 @@
       </c>
       <c r="AF400" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG400" t="n">
@@ -46789,7 +46789,7 @@
       </c>
       <c r="AF401" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG401" t="n">
@@ -46906,7 +46906,7 @@
       </c>
       <c r="AF402" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG402" t="n">
@@ -47019,7 +47019,7 @@
       </c>
       <c r="AF403" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG403" t="n">
@@ -47132,7 +47132,7 @@
       </c>
       <c r="AF404" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG404" t="n">
@@ -47362,7 +47362,7 @@
       </c>
       <c r="AF406" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG406" t="n">
@@ -47471,7 +47471,7 @@
       </c>
       <c r="AF407" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG407" t="n">
@@ -47701,7 +47701,7 @@
       </c>
       <c r="AF409" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG409" t="n">
@@ -47814,7 +47814,7 @@
       </c>
       <c r="AF410" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG410" t="n">
@@ -48040,7 +48040,7 @@
       </c>
       <c r="AF412" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG412" t="n">
@@ -48153,7 +48153,7 @@
       </c>
       <c r="AF413" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG413" t="n">
@@ -48270,7 +48270,7 @@
       </c>
       <c r="AF414" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG414" t="n">
@@ -48391,7 +48391,7 @@
       </c>
       <c r="AF415" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG415" t="n">
@@ -48508,7 +48508,7 @@
       </c>
       <c r="AF416" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG416" t="n">
@@ -48625,7 +48625,7 @@
       </c>
       <c r="AF417" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG417" t="n">
@@ -48734,7 +48734,7 @@
       </c>
       <c r="AF418" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG418" t="n">
@@ -48843,7 +48843,7 @@
       </c>
       <c r="AF419" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG419" t="n">
@@ -48952,7 +48952,7 @@
       </c>
       <c r="AF420" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG420" t="n">
@@ -49069,7 +49069,7 @@
       </c>
       <c r="AF421" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG421" t="n">
@@ -49182,7 +49182,7 @@
       </c>
       <c r="AF422" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG422" t="n">
@@ -49299,7 +49299,7 @@
       </c>
       <c r="AF423" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG423" t="n">
@@ -49416,7 +49416,7 @@
       </c>
       <c r="AF424" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG424" t="n">
@@ -49650,7 +49650,7 @@
       </c>
       <c r="AF426" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG426" t="n">
@@ -49880,7 +49880,7 @@
       </c>
       <c r="AF428" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG428" t="n">
@@ -49993,7 +49993,7 @@
       </c>
       <c r="AF429" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG429" t="n">
@@ -50106,7 +50106,7 @@
       </c>
       <c r="AF430" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG430" t="n">
@@ -50332,7 +50332,7 @@
       </c>
       <c r="AF432" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG432" t="n">
@@ -50796,7 +50796,7 @@
       </c>
       <c r="AF436" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG436" t="n">
@@ -51022,7 +51022,7 @@
       </c>
       <c r="AF438" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG438" t="n">
@@ -51369,7 +51369,7 @@
       </c>
       <c r="AF441" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG441" t="n">
@@ -51482,7 +51482,7 @@
       </c>
       <c r="AF442" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG442" t="n">
@@ -51595,7 +51595,7 @@
       </c>
       <c r="AF443" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG443" t="n">
@@ -51712,7 +51712,7 @@
       </c>
       <c r="AF444" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG444" t="n">
@@ -51821,7 +51821,7 @@
       </c>
       <c r="AF445" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG445" t="n">
@@ -51930,7 +51930,7 @@
       </c>
       <c r="AF446" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG446" t="n">
@@ -52152,7 +52152,7 @@
       </c>
       <c r="AF448" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG448" t="n">
@@ -52269,7 +52269,7 @@
       </c>
       <c r="AF449" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG449" t="n">
@@ -52604,7 +52604,7 @@
       </c>
       <c r="AF452" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG452" t="n">
@@ -52713,7 +52713,7 @@
       </c>
       <c r="AF453" t="inlineStr">
         <is>
-          <t>mineraloth</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG453" t="n">
@@ -52822,7 +52822,7 @@
       </c>
       <c r="AF454" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG454" t="n">
@@ -52935,7 +52935,7 @@
       </c>
       <c r="AF455" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG455" t="n">
@@ -53044,7 +53044,7 @@
       </c>
       <c r="AF456" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG456" t="n">
@@ -53157,7 +53157,7 @@
       </c>
       <c r="AF457" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG457" t="n">
@@ -53274,7 +53274,7 @@
       </c>
       <c r="AF458" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG458" t="n">
@@ -53508,7 +53508,7 @@
       </c>
       <c r="AF460" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG460" t="n">
@@ -53621,7 +53621,7 @@
       </c>
       <c r="AF461" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG461" t="n">
@@ -53734,7 +53734,7 @@
       </c>
       <c r="AF462" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG462" t="n">
@@ -53843,7 +53843,7 @@
       </c>
       <c r="AF463" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG463" t="n">
@@ -53956,7 +53956,7 @@
       </c>
       <c r="AF464" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG464" t="n">
@@ -54065,7 +54065,7 @@
       </c>
       <c r="AF465" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG465" t="n">
@@ -54182,7 +54182,7 @@
       </c>
       <c r="AF466" t="inlineStr">
         <is>
-          <t>oth</t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AG466" t="n">
@@ -54303,7 +54303,7 @@
       </c>
       <c r="AF467" t="inlineStr">
         <is>
-          <t>mineral</t>
+          <t>P2O5</t>
         </is>
       </c>
       <c r="AG467" t="n">

</xml_diff>